<commit_message>
Ajout draft mapping f595a2bd5e53be80aa00972cfd76eee4a5f7087b
</commit_message>
<xml_diff>
--- a/amelioration-mapping/ig/StructureDefinition-RORPractitionerRoleName.xlsx
+++ b/amelioration-mapping/ig/StructureDefinition-RORPractitionerRoleName.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="139">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-04T07:25:47+00:00</t>
+    <t>2024-03-12T09:15:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -264,9 +264,6 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
-    <t>ExerciceProfessionnel</t>
-  </si>
-  <si>
     <t>Extension.id</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>exerciseTitle</t>
   </si>
   <si>
-    <t>civiliteExercice : JDV-J208-CiviliteExercice-ROR</t>
-  </si>
-  <si>
     <t>Extension.extension:exerciseTitle.id</t>
   </si>
   <si>
@@ -400,46 +394,49 @@
     <t>https://mos.esante.gouv.fr/NOS/JDV_J208-CiviliteExercice-ROR/FHIR/JDV-J208-CiviliteExercice-ROR</t>
   </si>
   <si>
+    <t>civiliteExercice</t>
+  </si>
+  <si>
     <t>Extension.extension:exerciseLastName</t>
   </si>
   <si>
     <t>exerciseLastName</t>
   </si>
   <si>
+    <t>Extension.extension:exerciseLastName.id</t>
+  </si>
+  <si>
+    <t>Extension.extension:exerciseLastName.extension</t>
+  </si>
+  <si>
+    <t>Extension.extension:exerciseLastName.url</t>
+  </si>
+  <si>
+    <t>Extension.extension:exerciseLastName.value[x]</t>
+  </si>
+  <si>
     <t>nomExercice</t>
   </si>
   <si>
-    <t>Extension.extension:exerciseLastName.id</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseLastName.extension</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseLastName.url</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseLastName.value[x]</t>
-  </si>
-  <si>
     <t>Extension.extension:exerciseFirstName</t>
   </si>
   <si>
     <t>exerciseFirstName</t>
   </si>
   <si>
+    <t>Extension.extension:exerciseFirstName.id</t>
+  </si>
+  <si>
+    <t>Extension.extension:exerciseFirstName.extension</t>
+  </si>
+  <si>
+    <t>Extension.extension:exerciseFirstName.url</t>
+  </si>
+  <si>
+    <t>Extension.extension:exerciseFirstName.value[x]</t>
+  </si>
+  <si>
     <t>prenomExercice</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseFirstName.id</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseFirstName.extension</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseFirstName.url</t>
-  </si>
-  <si>
-    <t>Extension.extension:exerciseFirstName.value[x]</t>
   </si>
   <si>
     <t>base64Binary
@@ -1021,15 +1018,15 @@
         <v>76</v>
       </c>
       <c r="AL2" t="s" s="2">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1040,25 +1037,25 @@
         <v>77</v>
       </c>
       <c r="G3" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K3" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="H3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="L3" t="s" s="2">
+      <c r="M3" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>87</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1109,22 +1106,22 @@
         <v>76</v>
       </c>
       <c r="AF3" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AG3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH3" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI3" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ3" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK3" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AG3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH3" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK3" t="s" s="2">
-        <v>89</v>
       </c>
       <c r="AL3" t="s" s="2">
         <v>76</v>
@@ -1132,10 +1129,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1143,7 +1140,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>78</v>
@@ -1158,13 +1155,13 @@
         <v>76</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L4" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1203,19 +1200,19 @@
         <v>76</v>
       </c>
       <c r="AB4" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AC4" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="AC4" t="s" s="2">
+      <c r="AD4" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE4" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AD4" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE4" t="s" s="2">
+      <c r="AF4" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="AF4" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>77</v>
@@ -1238,13 +1235,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="D5" t="s" s="2">
         <v>76</v>
@@ -1254,7 +1251,7 @@
         <v>77</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>76</v>
@@ -1266,13 +1263,13 @@
         <v>76</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L5" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1323,7 +1320,7 @@
         <v>76</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>77</v>
@@ -1341,15 +1338,15 @@
         <v>76</v>
       </c>
       <c r="AL5" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1360,25 +1357,25 @@
         <v>77</v>
       </c>
       <c r="G6" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="H6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>87</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1429,22 +1426,22 @@
         <v>76</v>
       </c>
       <c r="AF6" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AG6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH6" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK6" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>89</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>76</v>
@@ -1452,10 +1449,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1478,13 +1475,13 @@
         <v>76</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1523,19 +1520,19 @@
         <v>76</v>
       </c>
       <c r="AB7" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AC7" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="AC7" t="s" s="2">
+      <c r="AD7" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE7" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AD7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE7" t="s" s="2">
+      <c r="AF7" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>77</v>
@@ -1558,10 +1555,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -1569,10 +1566,10 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>76</v>
@@ -1584,16 +1581,16 @@
         <v>76</v>
       </c>
       <c r="K8" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L8" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M8" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="N8" t="s" s="2">
         <v>107</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N8" t="s" s="2">
-        <v>109</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -1601,7 +1598,7 @@
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S8" t="s" s="2">
         <v>76</v>
@@ -1643,13 +1640,13 @@
         <v>76</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI8" t="s" s="2">
         <v>76</v>
@@ -1658,7 +1655,7 @@
         <v>76</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>76</v>
@@ -1666,10 +1663,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
@@ -1680,7 +1677,7 @@
         <v>77</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>76</v>
@@ -1692,13 +1689,13 @@
         <v>76</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="M9" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="L9" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>116</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1737,32 +1734,32 @@
         <v>76</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AC9" s="2"/>
       <c r="AD9" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI9" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>76</v>
@@ -1770,13 +1767,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s" s="2">
         <v>76</v>
@@ -1786,7 +1783,7 @@
         <v>77</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>76</v>
@@ -1798,13 +1795,13 @@
         <v>76</v>
       </c>
       <c r="K10" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="L10" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="M10" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="L10" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>116</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1831,11 +1828,11 @@
         <v>76</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Y10" s="2"/>
       <c r="Z10" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AA10" t="s" s="2">
         <v>76</v>
@@ -1853,46 +1850,46 @@
         <v>76</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>76</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s" s="2">
         <v>125</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>126</v>
       </c>
       <c r="D11" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>76</v>
@@ -1904,13 +1901,13 @@
         <v>76</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L11" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1961,7 +1958,7 @@
         <v>76</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>77</v>
@@ -1979,15 +1976,15 @@
         <v>76</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>127</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -1998,25 +1995,25 @@
         <v>77</v>
       </c>
       <c r="G12" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K12" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="H12" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I12" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J12" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K12" t="s" s="2">
+      <c r="L12" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="L12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>87</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2067,22 +2064,22 @@
         <v>76</v>
       </c>
       <c r="AF12" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH12" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK12" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>89</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>76</v>
@@ -2090,10 +2087,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2116,13 +2113,13 @@
         <v>76</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L13" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -2161,19 +2158,19 @@
         <v>76</v>
       </c>
       <c r="AB13" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AC13" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="AC13" t="s" s="2">
+      <c r="AD13" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE13" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AD13" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE13" t="s" s="2">
+      <c r="AF13" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="AF13" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>77</v>
@@ -2196,10 +2193,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2207,10 +2204,10 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>76</v>
@@ -2222,16 +2219,16 @@
         <v>76</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L14" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M14" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="N14" t="s" s="2">
         <v>107</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>109</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
@@ -2239,7 +2236,7 @@
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S14" t="s" s="2">
         <v>76</v>
@@ -2281,13 +2278,13 @@
         <v>76</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>76</v>
@@ -2296,7 +2293,7 @@
         <v>76</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>76</v>
@@ -2304,10 +2301,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -2318,25 +2315,25 @@
         <v>77</v>
       </c>
       <c r="G15" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I15" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J15" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="H15" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I15" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J15" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K15" t="s" s="2">
-        <v>85</v>
-      </c>
       <c r="L15" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -2387,36 +2384,36 @@
         <v>76</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>76</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s" s="2">
         <v>132</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="C16" t="s" s="2">
-        <v>133</v>
       </c>
       <c r="D16" t="s" s="2">
         <v>76</v>
@@ -2426,7 +2423,7 @@
         <v>77</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>76</v>
@@ -2438,13 +2435,13 @@
         <v>76</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L16" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -2495,7 +2492,7 @@
         <v>76</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>77</v>
@@ -2513,15 +2510,15 @@
         <v>76</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>134</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -2532,25 +2529,25 @@
         <v>77</v>
       </c>
       <c r="G17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="H17" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I17" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J17" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>87</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -2601,22 +2598,22 @@
         <v>76</v>
       </c>
       <c r="AF17" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>89</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>76</v>
@@ -2624,10 +2621,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -2650,13 +2647,13 @@
         <v>76</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L18" t="s" s="2">
         <v>29</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -2695,19 +2692,19 @@
         <v>76</v>
       </c>
       <c r="AB18" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AC18" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="AC18" t="s" s="2">
+      <c r="AD18" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE18" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AD18" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE18" t="s" s="2">
+      <c r="AF18" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="AF18" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>77</v>
@@ -2730,10 +2727,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -2741,10 +2738,10 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>76</v>
@@ -2756,16 +2753,16 @@
         <v>76</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M19" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>107</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>109</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -2773,7 +2770,7 @@
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S19" t="s" s="2">
         <v>76</v>
@@ -2815,13 +2812,13 @@
         <v>76</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>76</v>
@@ -2830,7 +2827,7 @@
         <v>76</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>76</v>
@@ -2838,10 +2835,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -2852,25 +2849,25 @@
         <v>77</v>
       </c>
       <c r="G20" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="H20" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I20" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J20" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="H20" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I20" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J20" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K20" t="s" s="2">
-        <v>85</v>
-      </c>
       <c r="L20" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -2921,33 +2918,33 @@
         <v>76</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>76</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -2955,10 +2952,10 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>76</v>
@@ -2970,16 +2967,16 @@
         <v>76</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>107</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>109</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3029,13 +3026,13 @@
         <v>76</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>76</v>
@@ -3044,7 +3041,7 @@
         <v>76</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>76</v>
@@ -3052,10 +3049,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3078,13 +3075,13 @@
         <v>76</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3135,22 +3132,22 @@
         <v>76</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>76</v>

</xml_diff>